<commit_message>
Work on ID IOOUT and merge to matlab instead of .out
</commit_message>
<xml_diff>
--- a/MEX/subs_called.xlsx
+++ b/MEX/subs_called.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="171027" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>SUBS</t>
   </si>
@@ -111,6 +114,9 @@
   </si>
   <si>
     <t xml:space="preserve">Rocket </t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -146,13 +152,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -160,66 +169,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -543,42 +492,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -586,177 +543,207 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B11">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C11">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B14">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
         <v>15</v>
-      </c>
-      <c r="B16">
-        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
         <v>16</v>
-      </c>
-      <c r="B17">
-        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
         <v>17</v>
-      </c>
-      <c r="B18">
-        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
         <v>18</v>
-      </c>
-      <c r="B19">
-        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1">
+    <filterColumn colId="1" showButton="0"/>
+    <sortState ref="A2:C28">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <conditionalFormatting sqref="B2:B28">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="1" priority="4">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update wrapper wrapper updated pour avoir le même format d'utilisation que la méthode MEX
</commit_message>
<xml_diff>
--- a/MEX/subs_called.xlsx
+++ b/MEX/subs_called.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27907"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Documents\GitHub\CEAMatlabAPI\MEX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rene/Cloud/Documents_Poly/Annee_2016-2017/H17/AER3900/CEA-Matlab-Integration/MEX/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="7600" yWindow="460" windowWidth="21200" windowHeight="15860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
   </definedNames>
-  <calcPr calcId="171027" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>SUBS</t>
   </si>
@@ -122,7 +128,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -495,16 +501,16 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -513,7 +519,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -524,7 +530,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -535,7 +541,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -543,7 +549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -554,7 +560,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -565,7 +571,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -576,7 +582,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -587,7 +593,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -598,7 +604,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -609,50 +615,62 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11">
-        <v>1411</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -660,7 +678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -668,15 +686,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -684,47 +705,50 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
ITS ALIVE!!!! okay now seriously, the cea2.mex function now works without writing a new file! the only output now is matlab struct
</commit_message>
<xml_diff>
--- a/MEX/subs_called.xlsx
+++ b/MEX/subs_called.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27907"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rene/Cloud/Documents_Poly/Annee_2016-2017/H17/AER3900/CEA-Matlab-Integration/MEX/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Documents\GitHub\CEAMatlabAPI\MEX\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="460" windowWidth="21200" windowHeight="15860"/>
+    <workbookView xWindow="7605" yWindow="465" windowWidth="21195" windowHeight="15855"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,18 +22,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>SUBS</t>
   </si>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -501,16 +501,16 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +519,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -530,7 +530,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -541,7 +541,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -549,7 +549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -560,7 +560,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -571,7 +571,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -582,7 +582,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -593,7 +593,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -604,7 +604,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -615,7 +615,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -626,7 +626,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -637,7 +637,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -648,7 +648,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -659,7 +659,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -670,23 +670,29 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -697,20 +703,23 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -718,37 +727,37 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>

</xml_diff>